<commit_message>
Update Growth of $10000 at compound interest rate.xlsx
</commit_message>
<xml_diff>
--- a/Growth of $10000 at compound interest rate.xlsx
+++ b/Growth of $10000 at compound interest rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maisk\Documents\Actuary\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D776494-B353-4BA0-B16B-524DE8295C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C47448-7C0D-4699-A1CE-1326CD594249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8AD88027-B163-47E5-BE50-26317B59B950}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Years</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Growth of $10,000 at Compound Interest Rate j_12</t>
+  </si>
+  <si>
+    <t>This excel file demonstrates how a $10,000 principal accumulates at different compound interest rates over time.</t>
   </si>
 </sst>
 </file>
@@ -101,13 +104,16 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -228,7 +234,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -261,7 +267,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$9:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
@@ -319,7 +325,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -352,7 +358,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$11</c:f>
+              <c:f>Sheet1!$C$9:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
@@ -410,7 +416,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -443,7 +449,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$11</c:f>
+              <c:f>Sheet1!$D$9:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
@@ -501,7 +507,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -534,7 +540,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$11</c:f>
+              <c:f>Sheet1!$E$9:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1446,13 +1452,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1778,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3C07FD-E0A5-4E4E-8AC5-3CDAA93E94DC}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1790,221 +1796,232 @@
     <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:5" ht="11.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B8" s="3">
         <v>0.06</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C8" s="3">
         <v>0.08</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D8" s="3">
         <v>0.1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E8" s="3">
         <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <f>$B$13*(1+B$3/12)^($A4*12)</f>
-        <v>13488.501525493037</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:E11" si="0">$B$13*(1+C$3/12)^($A4*12)</f>
-        <v>14898.457083016061</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>16453.089347785848</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>18166.966985640913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <f t="shared" ref="B5:B11" si="1">$B$13*(1+B$3/12)^($A5*12)</f>
-        <v>18193.967340322804</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>22196.402345447143</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>27070.41490862241</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>33003.8689457367</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1">
-        <f t="shared" si="1"/>
-        <v>24540.935622471461</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>33069.214774100132</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>44539.195517319844</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>59958.019753561799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <f t="shared" si="1"/>
-        <v>33102.044758073273</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>49268.027708097143</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>73280.736332496628</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>108925.5365387363</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <f t="shared" si="1"/>
-        <v>44649.698121621019</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>73401.75963739313</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>120569.45023501034</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>197884.66261924454</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="1"/>
-        <v>60225.752122628881</v>
+        <f>$B$18*(1+B$8/12)^($A9*12)</f>
+        <v>13488.501525493037</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>109357.2965775562</v>
+        <f t="shared" ref="C9:E16" si="0">$B$18*(1+C$8/12)^($A9*12)</f>
+        <v>14898.457083016061</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>198373.99373300443</v>
+        <v>16453.089347785848</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>359496.41327685065</v>
+        <v>18166.966985640913</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
-        <v>81235.514938004504</v>
+        <f t="shared" ref="B10:B16" si="1">$B$18*(1+B$8/12)^($A10*12)</f>
+        <v>18193.967340322804</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>162925.49897753802</v>
+        <v>22196.402345447143</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>326386.50431662303</v>
+        <v>27070.41490862241</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>653095.94714568695</v>
+        <v>33003.8689457367</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
-        <v>109574.53671654862</v>
+        <v>24540.935622471461</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>242733.85542458278</v>
+        <v>33069.214774100132</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>537006.63174328906</v>
+        <v>44539.195517319844</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>1186477.2510251577</v>
+        <v>59958.019753561799</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>33102.044758073273</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>49268.027708097143</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>73280.736332496628</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>108925.5365387363</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>44649.698121621019</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>73401.75963739313</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>120569.45023501034</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>197884.66261924454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="1"/>
+        <v>60225.752122628881</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>109357.2965775562</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>198373.99373300443</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>359496.41327685065</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>81235.514938004504</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>162925.49897753802</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>326386.50431662303</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>653095.94714568695</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="1"/>
+        <v>109574.53671654862</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>242733.85542458278</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>537006.63174328906</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>1186477.2510251577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B18" s="1">
         <v>10000</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:E2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>